<commit_message>
update later verion *.md and regenerating demo *.yaml files
</commit_message>
<xml_diff>
--- a/inputs/demo-paper-2017/排版示例-信息.xlsx
+++ b/inputs/demo-paper-2017/排版示例-信息.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="82">
   <si>
     <t>题型</t>
   </si>
@@ -108,12 +108,30 @@
     <t>S</t>
   </si>
   <si>
-    <t>P</t>
-  </si>
-  <si>
     <t>E</t>
   </si>
   <si>
+    <t>329</t>
+  </si>
+  <si>
+    <t>405</t>
+  </si>
+  <si>
+    <t>421</t>
+  </si>
+  <si>
+    <t>399</t>
+  </si>
+  <si>
+    <t>398</t>
+  </si>
+  <si>
+    <t>548</t>
+  </si>
+  <si>
+    <t>153</t>
+  </si>
+  <si>
     <t>Would a Work-Free World Be So Bad?</t>
   </si>
   <si>
@@ -174,7 +192,7 @@
     <t>2017-12-25</t>
   </si>
   <si>
-    <t>hhttps://www.theatlantic.com/business/archive/2016/06/would-a-world-without-work-be-so-bad/488711/</t>
+    <t>https://www.theatlantic.com/business/archive/2016/06/would-a-world-without-work-be-so-bad/488711/</t>
   </si>
   <si>
     <t>https://www.theguardian.com/commentisfree/2015/jul/05/the-guardian-view-on-the-olympic-legacy-running-out-of-steam</t>
@@ -665,20 +683,20 @@
       <c r="D2" t="s">
         <v>29</v>
       </c>
-      <c r="E2">
-        <v>329</v>
+      <c r="E2" t="s">
+        <v>31</v>
       </c>
       <c r="F2" t="s">
-        <v>32</v>
+        <v>38</v>
       </c>
       <c r="G2" t="s">
-        <v>39</v>
+        <v>45</v>
       </c>
       <c r="I2" t="s">
-        <v>45</v>
-      </c>
-      <c r="J2" t="s">
-        <v>52</v>
+        <v>51</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="3" spans="1:10">
@@ -694,17 +712,17 @@
       <c r="D3" t="s">
         <v>29</v>
       </c>
-      <c r="E3">
-        <v>405</v>
+      <c r="E3" t="s">
+        <v>32</v>
       </c>
       <c r="F3" t="s">
-        <v>33</v>
+        <v>39</v>
       </c>
       <c r="I3" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="4" spans="1:10">
@@ -718,22 +736,22 @@
         <v>25</v>
       </c>
       <c r="D4" t="s">
-        <v>30</v>
-      </c>
-      <c r="E4">
-        <v>421</v>
+        <v>29</v>
+      </c>
+      <c r="E4" t="s">
+        <v>33</v>
       </c>
       <c r="F4" t="s">
-        <v>34</v>
+        <v>40</v>
       </c>
       <c r="G4" t="s">
-        <v>40</v>
+        <v>46</v>
       </c>
       <c r="I4" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>54</v>
+        <v>60</v>
       </c>
     </row>
     <row r="5" spans="1:10">
@@ -747,22 +765,22 @@
         <v>26</v>
       </c>
       <c r="D5" t="s">
-        <v>31</v>
-      </c>
-      <c r="E5">
-        <v>399</v>
+        <v>30</v>
+      </c>
+      <c r="E5" t="s">
+        <v>34</v>
       </c>
       <c r="F5" t="s">
-        <v>35</v>
+        <v>41</v>
       </c>
       <c r="G5" t="s">
-        <v>41</v>
+        <v>47</v>
       </c>
       <c r="I5" t="s">
-        <v>48</v>
+        <v>54</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>55</v>
+        <v>61</v>
       </c>
     </row>
     <row r="6" spans="1:10">
@@ -778,20 +796,20 @@
       <c r="D6" t="s">
         <v>29</v>
       </c>
-      <c r="E6">
-        <v>398</v>
+      <c r="E6" t="s">
+        <v>35</v>
       </c>
       <c r="F6" t="s">
-        <v>36</v>
+        <v>42</v>
       </c>
       <c r="G6" t="s">
-        <v>42</v>
+        <v>48</v>
       </c>
       <c r="I6" t="s">
-        <v>49</v>
+        <v>55</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>56</v>
+        <v>62</v>
       </c>
     </row>
     <row r="7" spans="1:10">
@@ -804,20 +822,20 @@
       <c r="C7" t="s">
         <v>28</v>
       </c>
-      <c r="E7">
-        <v>548</v>
+      <c r="E7" t="s">
+        <v>36</v>
       </c>
       <c r="F7" t="s">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="G7" t="s">
-        <v>43</v>
+        <v>49</v>
       </c>
       <c r="I7" t="s">
-        <v>50</v>
+        <v>56</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>57</v>
+        <v>63</v>
       </c>
     </row>
     <row r="8" spans="1:10">
@@ -827,30 +845,31 @@
       <c r="B8" t="s">
         <v>22</v>
       </c>
-      <c r="E8">
-        <v>153</v>
+      <c r="E8" t="s">
+        <v>37</v>
       </c>
       <c r="F8" t="s">
-        <v>38</v>
+        <v>44</v>
       </c>
       <c r="G8" t="s">
-        <v>44</v>
+        <v>50</v>
       </c>
       <c r="I8" t="s">
-        <v>51</v>
+        <v>57</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>58</v>
+        <v>64</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="J3" r:id="rId1"/>
-    <hyperlink ref="J4" r:id="rId2"/>
-    <hyperlink ref="J5" r:id="rId3"/>
-    <hyperlink ref="J6" r:id="rId4"/>
-    <hyperlink ref="J7" r:id="rId5"/>
-    <hyperlink ref="J8" r:id="rId6"/>
+    <hyperlink ref="J2" r:id="rId1"/>
+    <hyperlink ref="J3" r:id="rId2"/>
+    <hyperlink ref="J4" r:id="rId3"/>
+    <hyperlink ref="J5" r:id="rId4"/>
+    <hyperlink ref="J6" r:id="rId5"/>
+    <hyperlink ref="J7" r:id="rId6"/>
+    <hyperlink ref="J8" r:id="rId7"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -866,34 +885,34 @@
   <sheetData>
     <row r="1" spans="1:10">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>60</v>
+        <v>66</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>61</v>
+        <v>67</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>62</v>
+        <v>68</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>63</v>
+        <v>69</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>64</v>
+        <v>70</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>65</v>
+        <v>71</v>
       </c>
       <c r="H1" s="1" t="s">
-        <v>66</v>
+        <v>72</v>
       </c>
       <c r="I1" s="1" t="s">
-        <v>67</v>
+        <v>73</v>
       </c>
       <c r="J1" s="1" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
     </row>
     <row r="2" spans="1:10">
@@ -966,7 +985,7 @@
     </row>
     <row r="6" spans="1:10">
       <c r="A6" t="s">
-        <v>68</v>
+        <v>74</v>
       </c>
       <c r="B6">
         <v>9</v>
@@ -1011,31 +1030,31 @@
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="1" t="s">
-        <v>59</v>
+        <v>65</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>69</v>
+        <v>75</v>
       </c>
       <c r="C1" s="1" t="s">
-        <v>70</v>
+        <v>76</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>71</v>
+        <v>77</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>72</v>
+        <v>78</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>73</v>
+        <v>79</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="I1" s="1" t="s">
         <v>74</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>75</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:9">

</xml_diff>